<commit_message>
Added part of 2nd example
</commit_message>
<xml_diff>
--- a/2_Formulas_and_Functions/7_Text_Functions/1_Text_Functions.xlsx
+++ b/2_Formulas_and_Functions/7_Text_Functions/1_Text_Functions.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\2_Formulas_and_Functions\7_Text_Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1153069E-67B7-4960-BA45-07EEAB841371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D281E561-51B8-41A1-834F-50F127D620C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
   <si>
     <t>Employee Name</t>
   </si>
@@ -51,9 +52,6 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Address Line 1</t>
-  </si>
-  <si>
     <t>City, State, Zip Code</t>
   </si>
   <si>
@@ -121,6 +119,27 @@
   </si>
   <si>
     <t>Houston, TX 45688</t>
+  </si>
+  <si>
+    <t>123 MAIN STREET, APARTMENT A1 NEW YORK, NY 12345</t>
+  </si>
+  <si>
+    <t>123 CENTER STREET NEW YORK, NY 12345</t>
+  </si>
+  <si>
+    <t>123 LAKE BLVD, HOUSE B HOUSTON, TX 45688</t>
+  </si>
+  <si>
+    <t>sjones@company.com</t>
+  </si>
+  <si>
+    <t>ajohnson@company.com</t>
+  </si>
+  <si>
+    <t>Ashley Johnson</t>
+  </si>
+  <si>
+    <t>Area Code</t>
   </si>
 </sst>
 </file>
@@ -166,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,18 +208,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -482,37 +513,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.42578125" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{F8C5DD9A-601D-4CBB-BD17-1989BBBF60D3}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{CDE7D0CA-136C-452F-9500-11B3645E3C83}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{73CF4A30-1B5F-4E9D-8BF7-69EBE10AA00B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -521,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72D6549-25C9-4BA9-93D0-EF0CE96AE1DE}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F4" sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,42 +655,42 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,D2,E2)</f>
@@ -609,22 +711,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G4" si="0">_xlfn.TEXTJOIN(" ",TRUE,D3,E3)</f>
@@ -645,22 +747,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -687,4 +789,115 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770DD524-EA3D-430A-B599-F95058BF5B1F}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6FCC7C81-D583-44F5-BFA5-7BA33869A0BD}"/>
+    <hyperlink ref="C3" r:id="rId2" display="SJones@company.com" xr:uid="{793A5595-AAD9-494F-B6CF-7434040BB240}"/>
+    <hyperlink ref="C4" r:id="rId3" display="Ajohnson@company.com" xr:uid="{947F5469-9A22-4B4A-A47A-17411AE02A5E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>